<commit_message>
Adds state to initial screen
</commit_message>
<xml_diff>
--- a/Resultado.xlsx
+++ b/Resultado.xlsx
@@ -14,12 +14,13 @@
     <sheet name="Limpeza (volume)" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Limpeza (outros)" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Outros" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Bandeirantes" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Bob" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Taquaral" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="São Vicente" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Guará" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="São Vicente" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Taquaral" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Bandeirantes" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Guará" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Bob" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Ponte Preta" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Resultados Gerais" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,16 +464,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Supermercado</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Turno</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>Quantidade</t>
         </is>
       </c>
@@ -491,27 +482,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Ponte Preta</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
+      <c r="D2" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7622210571816</v>
+        <v>12240900</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Suco (18g)</t>
+          <t>molho de tomate 300g</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -519,27 +500,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
+      <c r="D3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7896584300079</v>
+        <v>7896292333000</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Molho de Tomate (300g)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,27 +518,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>6</v>
+      <c r="D4" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7891095300372</v>
+        <v>7896894900068</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Farinha de Mandioca (500g)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -575,27 +536,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
+      <c r="D5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7896894900013</v>
+        <v>7896045110582</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Açúcar (1kg)</t>
+          <t>Achocolatado (370g)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -603,27 +554,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7891000376881</v>
+        <v>7896080841403</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Biscoito recheado (90g)</t>
+          <t>Macarrão (200g)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -631,27 +572,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7896584300352</v>
+        <v>7896205789450</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Arroz (1kg)</t>
+          <t xml:space="preserve">macarrão </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -659,27 +590,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>5</v>
+      <c r="D8" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7891910000197</v>
+        <v>7891032014621</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Açúcar (1kg)</t>
+          <t>Molho de Tomate (300g)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -687,27 +608,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>8</v>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7898949924180</v>
+        <v>7891095300372</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">feijão </t>
+          <t>Farinha de Mandioca (500g)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -715,27 +626,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Taquaral</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>25</v>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7896005202074</v>
+        <v>7622210571816</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Farinha de Trigo (1kg)</t>
+          <t>Suco (18g)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -743,27 +644,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Bandeirantes</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>8</v>
+      <c r="D11" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7897517206338</v>
+        <v>7896327512615</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Extrato de tomate (190g)</t>
+          <t>Amido de Milho (200g)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -771,27 +662,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
+      <c r="D12" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7896200115346</v>
+        <v>7896005286593</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Macarrão (500g)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -799,27 +680,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Bandeirantes</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>9</v>
+      <c r="D13" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7896894900068</v>
+        <v>7896005202074</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Açúcar (1kg)</t>
+          <t>Farinha de Trigo (1kg)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -827,27 +698,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>2</v>
+      <c r="D14" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>7891048050668</v>
+        <v>7896584300352</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Gelatina (20g)</t>
+          <t>Arroz (1kg)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -855,27 +716,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>4</v>
+      <c r="D15" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7896327512615</v>
+        <v>7891910000197</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Amido de Milho (200g)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -883,27 +734,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
+      <c r="D16" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7896005275399</v>
+        <v>7897517206338</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Macarrão (500g)</t>
+          <t>Extrato de tomate (190g)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -911,27 +752,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>8</v>
+      <c r="D17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>7896205789450</v>
+        <v>7896584300079</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">macarrão </t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -939,27 +770,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Taquaral</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>15</v>
+      <c r="D18" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7896005286593</v>
+        <v>7896200115346</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Macarrão (500g)</t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -967,23 +788,13 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>18</v>
+      <c r="D19" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>7896584300079</v>
+        <v>7896006744115</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -995,27 +806,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
+      <c r="D20" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>7896080841403</v>
+        <v>7896005275399</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Macarrão (200g)</t>
+          <t>Macarrão (500g)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1023,27 +824,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>1</v>
+      <c r="D21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>7896045110582</v>
+        <v>7898949924180</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Achocolatado (370g)</t>
+          <t xml:space="preserve">feijão </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1051,27 +842,17 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
+      <c r="D22" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>12240900</v>
+        <v>7891000376881</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>molho de tomate 300g</t>
+          <t>Biscoito recheado (90g)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1079,17 +860,7 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Guará</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
+      <c r="D23" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1107,83 +878,53 @@
           <t>Alimentos (peso)</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Ponte Preta</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2º TURNO: 12h às 14h</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>10</v>
+      <c r="D24" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>7896292333000</v>
+        <v>7896051111016</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Molho de Tomate (300g)</t>
+          <t xml:space="preserve">Leite 1L </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Alimentos (peso)</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Taquaral</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>14</v>
+          <t>Alimentos (volume)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>7891032014621</v>
+        <v>7898215151708</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Molho de Tomate (300g)</t>
+          <t>Leite (1L)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Alimentos (peso)</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
+          <t>Alimentos (volume)</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>7898247780297</v>
+        <v>7891107101621</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">óleo </t>
+          <t>Óleo (900mL)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1191,27 +932,17 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Taquaral</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2º TURNO: 12h às 14h</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>5</v>
+      <c r="D27" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7896051111016</v>
+        <v>7896036090244</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leite 1L </t>
+          <t>Óleo (900mL)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1219,27 +950,17 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Ponte Preta</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>11</v>
+      <c r="D28" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>7898215151708</v>
+        <v>7898247780297</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Leite (1L)</t>
+          <t xml:space="preserve">óleo </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1247,27 +968,17 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Bandeirantes</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>37</v>
+      <c r="D29" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>7896036090244</v>
+        <v>7986051111016</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Óleo (900mL)</t>
+          <t>Leite (1L)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1275,23 +986,13 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>10</v>
+      <c r="D30" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>7898215151708</v>
+        <v>7898080640611</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1303,27 +1004,17 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Guará</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>26</v>
+      <c r="D31" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7891107101621</v>
+        <v>7896256601848</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Óleo (900mL)</t>
+          <t>Leite (1L)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1331,293 +1022,111 @@
           <t>Alimentos (volume)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Guará</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>3</v>
+      <c r="D32" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7898215151708</v>
+        <v>7896104996393</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Leite (1L)</t>
+          <t>Papel Higiênico (12un)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Alimentos (volume)</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v>4</v>
+          <t>Limpeza (outros)</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7891107101621</v>
+        <v>7896060401818</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Óleo (900mL)</t>
+          <t>Sabão em pó (800g)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Alimentos (volume)</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
+          <t>Limpeza (peso)</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>7986051111016</v>
+        <v>7891528029498</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Leite (1L)</t>
+          <t>Pasta de Dente (70g)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Alimentos (volume)</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
+          <t>Limpeza (peso)</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>7898080640611</v>
+        <v>7891176117455</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Leite (1L)</t>
+          <t>Sabonete (85g)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Alimentos (volume)</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Taquaral</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>2º TURNO: 12h às 14h</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>7</v>
+          <t>Limpeza (peso)</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>7896104996393</v>
+        <v>7897664171701</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Papel Higiênico (12un)</t>
+          <t>Sabonete (85g)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Limpeza (outros)</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>1</v>
+          <t>Limpeza (peso)</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7891528029498</v>
+        <v>7891022638004</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Pasta de Dente (70g)</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Limpeza (peso)</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>7891176117455</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Sabonete (85g)</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Limpeza (peso)</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>7897664171701</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Sabonete (85g)</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Limpeza (peso)</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>7896060401818</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Sabão em pó (800g)</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Limpeza (peso)</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>7891022638004</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
           <t>Detergente (500mL)</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>São Vicente</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1632,7 +1141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1660,22 +1169,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Leite (1L)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2º TURNO: 12h às 14h</t>
+          <t>1º TURNO: 10h às 12h</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Molho de Tomate (300g)</t>
+          <t>Farinha de Trigo (1kg)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1684,13 +1193,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">feijão </t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1699,13 +1208,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">macarrão </t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1714,22 +1223,52 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">óleo </t>
+          <t>Leite (1L)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2º TURNO: 12h às 14h</t>
+          <t>1º TURNO: 10h às 12h</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Macarrão (500g)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Leite (1L)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1738,387 +1277,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Item</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Turno</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Quantidade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Açúcar (1kg)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Açúcar (1kg)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Detergente (500mL)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Farinha de Mandioca (500g)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Gelatina (20g)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Leite (1L)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Macarrão (500g)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Óleo (900mL)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Óleo (900mL)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Papel Higiênico (12un)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Pasta de Dente (70g)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Sabonete (85g)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Arroz (1kg)</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Molho de Tomate (300g)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Feijão (1kg)</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1º TURNO: 10h às 12h</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Feijão (1kg)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Extrato de tomate (190g)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Suco (18g)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Leite (1L)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Biscoito recheado (90g)</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Achocolatado (370g)</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Sabão em pó (800g)</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Macarrão (200g)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>4º TURNO: 16h às 18h</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2191,6 +1349,102 @@
         </is>
       </c>
       <c r="C4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Turno</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Açúcar (1kg)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Macarrão (500g)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sabonete (85g)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Amido de Milho (200g)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2280,13 +1534,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2297,6 +1551,77 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Quantidade de produtos</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade de códigos de barras</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Soma de peso de alimentos (kg)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Soma de volume de alimentos (L)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Soma de peso de produtos de limpeza (kg)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Soma de volume de produtos de limpeza (L)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>335</v>
+      </c>
+      <c r="B2" t="n">
+        <v>37</v>
+      </c>
+      <c r="C2" t="n">
+        <v>99.964</v>
+      </c>
+      <c r="D2" t="n">
+        <v>110.6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
           <t>Item</t>
         </is>
       </c>
@@ -2349,11 +1674,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Bandeirantes</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2364,17 +1689,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Farinha de Mandioca (500g)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2383,28 +1708,28 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Farinha de Trigo (1kg)</t>
+          <t>Farinha de Mandioca (500g)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bandeirantes</t>
+          <t>São Vicente</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Farinha de Trigo (1kg)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2413,58 +1738,58 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gelatina (20g)</t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ponte Preta</t>
+          <t>Bandeirantes</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gelatina (20g)</t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Bandeirantes</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Macarrão (500g)</t>
+          <t>Gelatina (20g)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Ponte Preta</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Macarrão (500g)</t>
+          <t>Gelatina (20g)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2473,43 +1798,43 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Amido de Milho (200g)</t>
+          <t>Macarrão (500g)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Bandeirantes</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Arroz (1kg)</t>
+          <t>Macarrão (500g)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Molho de Tomate (300g)</t>
+          <t>Macarrão (500g)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2518,28 +1843,28 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Amido de Milho (200g)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Arroz (1kg)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2548,7 +1873,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -2559,97 +1884,97 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Taquaral</t>
+          <t>São Vicente</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">feijão </t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Taquaral</t>
+          <t>São Vicente</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">macarrão </t>
+          <t>Feijão (1kg)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Taquaral</t>
+          <t>São Vicente</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>molho de tomate 300g</t>
+          <t>Molho de Tomate (300g)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Guará</t>
+          <t>Taquaral</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Extrato de tomate (190g)</t>
+          <t xml:space="preserve">feijão </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Taquaral</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Suco (18g)</t>
+          <t xml:space="preserve">macarrão </t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Taquaral</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Biscoito recheado (90g)</t>
+          <t>molho de tomate 300g</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>São Vicente</t>
+          <t>Guará</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -2659,7 +1984,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Achocolatado (370g)</t>
+          <t>Extrato de tomate (190g)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2668,21 +1993,66 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Suco (18g)</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>São Vicente</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Biscoito recheado (90g)</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>São Vicente</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Achocolatado (370g)</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>São Vicente</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>Macarrão (200g)</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>São Vicente</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C29" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2697,7 +2067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2870,6 +2240,21 @@
       </c>
       <c r="C11" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Leite (1L)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bandeirantes</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3117,7 +2502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3145,22 +2530,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Farinha de Trigo (1kg)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1º TURNO: 10h às 12h</t>
+          <t>4º TURNO: 16h às 18h</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Feijão (1kg)</t>
+          <t>Açúcar (1kg)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3169,22 +2554,322 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Detergente (500mL)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Farinha de Mandioca (500g)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Gelatina (20g)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Leite (1L)</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>1º TURNO: 10h às 12h</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>37</v>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Macarrão (500g)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Óleo (900mL)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Óleo (900mL)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Papel Higiênico (12un)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Pasta de Dente (70g)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sabonete (85g)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Arroz (1kg)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Molho de Tomate (300g)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Feijão (1kg)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1º TURNO: 10h às 12h</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Feijão (1kg)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Extrato de tomate (190g)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Suco (18g)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Leite (1L)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Biscoito recheado (90g)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Achocolatado (370g)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Sabão em pó (800g)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Macarrão (200g)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>4º TURNO: 16h às 18h</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3198,7 +2883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3226,22 +2911,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Açúcar (1kg)</t>
+          <t>Leite (1L)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1º TURNO: 10h às 12h</t>
+          <t>2º TURNO: 12h às 14h</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Macarrão (500g)</t>
+          <t>Molho de Tomate (300g)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3250,13 +2935,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sabonete (85g)</t>
+          <t xml:space="preserve">feijão </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3265,13 +2950,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Amido de Milho (200g)</t>
+          <t xml:space="preserve">macarrão </t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3280,7 +2965,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">óleo </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2º TURNO: 12h às 14h</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>